<commit_message>
updated graphs, included copy-sign ratings and summarising task data
</commit_message>
<xml_diff>
--- a/data/combined-data-tables/2022-03-11_lg-bg-demographics.xlsx
+++ b/data/combined-data-tables/2022-03-11_lg-bg-demographics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\freya\Desktop\PhD\3 SLI-Aptitude\data\combined-data-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA32284-EFE9-4FF3-BA78-642EF8DE1545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558A1995-C678-4E7E-8AA5-CB9ED2AF453A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1293,9 +1293,9 @@
   </sheetPr>
   <dimension ref="A1:BG34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T2" activeCellId="2" sqref="T11:T12 T8:T9 T2:T6"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1742,7 +1742,9 @@
       <c r="Q4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="2"/>
+      <c r="R4" s="2">
+        <v>2</v>
+      </c>
       <c r="S4" s="3">
         <v>16</v>
       </c>
@@ -1840,7 +1842,9 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="R5" s="2">
+        <v>1</v>
+      </c>
       <c r="S5" s="9">
         <v>17</v>
       </c>
@@ -1920,7 +1924,9 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="R6" s="2">
+        <v>1</v>
+      </c>
       <c r="S6" s="9">
         <v>18</v>
       </c>
@@ -2008,7 +2014,9 @@
       <c r="Q7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="R7" s="2"/>
+      <c r="R7" s="2">
+        <v>5</v>
+      </c>
       <c r="S7" s="3">
         <v>3</v>
       </c>
@@ -2100,7 +2108,9 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
+      <c r="R8" s="2">
+        <v>2</v>
+      </c>
       <c r="S8" s="3">
         <v>29</v>
       </c>
@@ -2390,7 +2400,9 @@
       <c r="Q11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="R11" s="2"/>
+      <c r="R11" s="2">
+        <v>1</v>
+      </c>
       <c r="S11" s="3">
         <v>18</v>
       </c>

</xml_diff>